<commit_message>
updated lab tests, as product
</commit_message>
<xml_diff>
--- a/updated_api_endpoints.xlsx
+++ b/updated_api_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\adv8\adv8_labOwners\labOwners3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6BE4A0-B06A-4AE9-877B-00CEB87F5797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1ECA5F-349B-4F8B-95A5-2249CA26DC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
   <si>
     <t>API Name</t>
   </si>
@@ -194,54 +194,6 @@
   </si>
   <si>
     <t>{bookingsLog:[{image,patientName,TestName,status,time}], inOutTrack:[{image,patientName,TestName,time}], missedOut:[{image,patientName,TestName,time}]}</t>
-  </si>
-  <si>
-    <t>lab-dashboard-testOffered</t>
-  </si>
-  <si>
-    <t>{
-  "tests": [
-    {
-      "name": "Blood Test",
-      "description": "Complete blood count",
-      "sampleName": "Blood",
-      "sampleType": "Venous",
-      "vialName": "EDTA Tube",
-      "preparationTime": "30 minutes",
-      "price": "1300",
-      "sampleCollection": ["Home", "At Lab"],
-      "availability": ["Monday", "Wednesday", "Friday"],
-      "features": ["Express Service", "Online Reports"],
-      "availableTimeSlots": ["9AM - 10AM", "10AM - 11AM", "11AM - 12PM"]
-    },
-    {
-      "name": "Urine Analysis",
-      "description": "Urinalysis test",
-      "sampleName": "Urine",
-      "sampleType": "Random",
-      "vialName": "Sterile Container",
-      "preparationTime": "15 minutes",
-      "price": "500",
-      "sampleCollection": ["At Lab"],
-      "availability": ["Monday", "Tuesday", "Thursday"],
-      "features": ["Online Reports"],
-      "availableTimeSlots": ["9AM - 10AM", "11AM - 12PM", "1PM - 2PM"]
-    },
-    {
-      "name": "X-Ray",
-      "description": "Chest X-ray",
-      "sampleName": "N/A",
-      "sampleType": "N/A",
-      "vialName": "N/A",
-      "preparationTime": "10 minutes",
-      "price": "1100",
-      "sampleCollection": ["At Lab"],
-      "availability": ["Monday", "Wednesday", "Friday"],
-      "features": ["Express Service"],
-      "availableTimeSlots": ["10AM - 11AM", "2PM - 3PM", "4PM - 5PM"]
-    }
-  ]
-}</t>
   </si>
   <si>
     <t>YES (1)</t>
@@ -342,6 +294,37 @@
   });</t>
     </r>
   </si>
+  <si>
+    <t>{
+  "labRef": "labID"
+  "productList": [
+    {
+      "name": "Blood Test",
+      "description": "Complete blood count",
+      ...
+    },
+    {
+      "name": "Urine Analysis",
+      "description": "Urinalysis test",
+    ...
+    },
+    {
+      "name": "X-Ray",
+      "description": "Chest X-ray",
+     ......
+    }
+  ]
+}</t>
+  </si>
+  <si>
+    <t>Yes, opened as of now</t>
+  </si>
+  <si>
+    <t>/api/product</t>
+  </si>
+  <si>
+    <t>updatedProduct JSON with ID</t>
+  </si>
 </sst>
 </file>
 
@@ -379,12 +362,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -425,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -438,17 +427,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H35"/>
+  <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -713,8 +708,8 @@
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>47</v>
+      <c r="H2" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:8">
@@ -726,7 +721,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:8" ht="90">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -744,7 +739,7 @@
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="6"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
@@ -758,7 +753,7 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="6"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
@@ -774,7 +769,7 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="6"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
@@ -790,7 +785,7 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="6"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
@@ -806,7 +801,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="90">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -815,8 +810,8 @@
       <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>48</v>
+      <c r="E10" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>22</v>
@@ -826,7 +821,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="60">
-      <c r="B11" s="6"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
@@ -844,7 +839,7 @@
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="6"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
@@ -862,7 +857,7 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="6"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
@@ -878,7 +873,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="240">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -896,7 +891,7 @@
       </c>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="6"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
@@ -910,7 +905,7 @@
       </c>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="6"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
@@ -926,7 +921,7 @@
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="6"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
@@ -940,7 +935,7 @@
       </c>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="6"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="3" t="s">
         <v>36</v>
       </c>
@@ -954,7 +949,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="300">
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -970,12 +965,12 @@
       <c r="G21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>46</v>
+      <c r="H21" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="6"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="3" t="s">
         <v>11</v>
       </c>
@@ -987,10 +982,10 @@
       <c r="G22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="7"/>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="6"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1004,10 +999,10 @@
       <c r="G23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="7"/>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="6"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="3" t="s">
         <v>35</v>
       </c>
@@ -1019,10 +1014,10 @@
       <c r="G24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="7"/>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="6"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="3" t="s">
         <v>36</v>
       </c>
@@ -1034,10 +1029,10 @@
       <c r="G25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H25" s="7"/>
+      <c r="H25" s="3"/>
     </row>
     <row r="28" spans="2:8" ht="225">
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1046,19 +1041,19 @@
       <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>49</v>
+      <c r="E28" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="7" t="s">
-        <v>46</v>
+      <c r="H28" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="6"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="3" t="s">
         <v>11</v>
       </c>
@@ -1072,7 +1067,7 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="6"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1088,7 +1083,7 @@
       </c>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="6"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="3" t="s">
         <v>35</v>
       </c>
@@ -1102,7 +1097,7 @@
       </c>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="6"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="3" t="s">
         <v>36</v>
       </c>
@@ -1115,7 +1110,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:7">
       <c r="B33" t="s">
         <v>40</v>
       </c>
@@ -1123,7 +1118,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:7">
       <c r="B34" t="s">
         <v>42</v>
       </c>
@@ -1131,16 +1126,75 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="409.5">
-      <c r="B35" t="s">
-        <v>44</v>
+    <row r="35" spans="2:7" ht="300">
+      <c r="B35" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="11"/>
+      <c r="C36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="11"/>
+      <c r="C37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="11"/>
+      <c r="C38" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="11"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B35:B39"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B15:B19"/>

</xml_diff>

<commit_message>
lab get is fixed
</commit_message>
<xml_diff>
--- a/updated_api_endpoints.xlsx
+++ b/updated_api_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\adv8\adv8_labOwners\labOwners3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1ECA5F-349B-4F8B-95A5-2249CA26DC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2351635F-65D2-40AE-9A44-07B40715A46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,16 +433,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -721,7 +721,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:8" ht="90">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -739,7 +739,7 @@
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="8"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
@@ -753,7 +753,7 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="8"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
@@ -769,7 +769,7 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="8"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
@@ -785,7 +785,7 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="8"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
@@ -801,7 +801,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="90">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -821,7 +821,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="60">
-      <c r="B11" s="8"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
@@ -839,7 +839,7 @@
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="8"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
@@ -857,7 +857,7 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="8"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
@@ -873,7 +873,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="240">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -891,7 +891,7 @@
       </c>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="8"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
@@ -905,7 +905,7 @@
       </c>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="8"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
@@ -921,7 +921,7 @@
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="8"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
@@ -935,7 +935,7 @@
       </c>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="8"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="3" t="s">
         <v>36</v>
       </c>
@@ -949,7 +949,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="300">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -970,7 +970,7 @@
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="8"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="3" t="s">
         <v>11</v>
       </c>
@@ -985,7 +985,7 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="8"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1002,7 +1002,7 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="8"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="3" t="s">
         <v>35</v>
       </c>
@@ -1017,7 +1017,7 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="8"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="3" t="s">
         <v>36</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="H25" s="3"/>
     </row>
     <row r="28" spans="2:8" ht="225">
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1053,7 +1053,7 @@
       </c>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="8"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="3" t="s">
         <v>11</v>
       </c>
@@ -1067,7 +1067,7 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="8"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1083,7 +1083,7 @@
       </c>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="8"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="3" t="s">
         <v>35</v>
       </c>
@@ -1097,7 +1097,7 @@
       </c>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="8"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="3" t="s">
         <v>36</v>
       </c>
@@ -1127,21 +1127,21 @@
       </c>
     </row>
     <row r="35" spans="2:7" ht="300">
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="9" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="11"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="3" t="s">
         <v>11</v>
       </c>
@@ -1155,7 +1155,7 @@
       </c>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="11"/>
+      <c r="B37" s="10"/>
       <c r="C37" s="3" t="s">
         <v>7</v>
       </c>
@@ -1171,7 +1171,7 @@
       </c>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="11"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="3" t="s">
         <v>35</v>
       </c>
@@ -1185,7 +1185,7 @@
       </c>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="11"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>

</xml_diff>

<commit_message>
new API for labOwners list added
</commit_message>
<xml_diff>
--- a/updated_api_endpoints.xlsx
+++ b/updated_api_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\adv8\adv8_labOwners\labOwners3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2351635F-65D2-40AE-9A44-07B40715A46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F73B1F0-5BA6-4072-AD05-4F97F615E74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="55">
   <si>
     <t>API Name</t>
   </si>
@@ -325,17 +325,33 @@
   <si>
     <t>updatedProduct JSON with ID</t>
   </si>
+  <si>
+    <t>/getlab/owner</t>
+  </si>
+  <si>
+    <t>Loggedin owners labs will be returned</t>
+  </si>
+  <si>
+    <t>Will be implemented after lab onboarding and booking process starts</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -362,7 +378,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,8 +391,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -410,13 +432,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -427,10 +499,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -442,7 +514,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -672,17 +770,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H39"/>
+  <dimension ref="B2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63.140625" customWidth="1"/>
     <col min="6" max="6" width="44" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
@@ -721,7 +819,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:8" ht="90">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -739,7 +837,7 @@
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="11"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
@@ -753,7 +851,7 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="11"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
@@ -769,7 +867,7 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="11"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
@@ -785,7 +883,7 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="11"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
@@ -801,7 +899,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="90">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -821,7 +919,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="60">
-      <c r="B11" s="11"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
@@ -839,7 +937,7 @@
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="11"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
@@ -857,7 +955,7 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="11"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
@@ -873,7 +971,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="240">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -891,7 +989,7 @@
       </c>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="11"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
@@ -905,7 +1003,7 @@
       </c>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="11"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
@@ -921,7 +1019,7 @@
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="11"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
@@ -935,7 +1033,7 @@
       </c>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="11"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="3" t="s">
         <v>36</v>
       </c>
@@ -949,7 +1047,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="300">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -970,7 +1068,7 @@
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="11"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="3" t="s">
         <v>11</v>
       </c>
@@ -985,7 +1083,7 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="11"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1002,7 +1100,7 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="11"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="3" t="s">
         <v>35</v>
       </c>
@@ -1017,7 +1115,7 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="11"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="3" t="s">
         <v>36</v>
       </c>
@@ -1032,10 +1130,10 @@
       <c r="H25" s="3"/>
     </row>
     <row r="28" spans="2:8" ht="225">
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -1054,7 +1152,7 @@
     </row>
     <row r="29" spans="2:8">
       <c r="B29" s="11"/>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -1068,7 +1166,7 @@
     </row>
     <row r="30" spans="2:8">
       <c r="B30" s="11"/>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -1084,7 +1182,7 @@
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="11"/>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -1098,108 +1196,140 @@
     </row>
     <row r="32" spans="2:8">
       <c r="B32" s="11"/>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="3" t="s">
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
-      <c r="B33" t="s">
+    <row r="33" spans="2:8">
+      <c r="B33" s="11"/>
+      <c r="C33" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="75">
+      <c r="B34" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E33" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="2:7">
-      <c r="B34" t="s">
+      <c r="F34" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+    </row>
+    <row r="35" spans="2:8" ht="45">
+      <c r="B35" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E34" t="s">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" ht="300">
-      <c r="B35" s="10" t="s">
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+    </row>
+    <row r="36" spans="2:8" ht="300">
+      <c r="B36" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F36" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G36" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="2:7">
-      <c r="B36" s="10"/>
-      <c r="C36" s="3" t="s">
+    <row r="37" spans="2:8">
+      <c r="B37" s="11"/>
+      <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7">
-      <c r="B37" s="10"/>
-      <c r="C37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
-      <c r="B38" s="10"/>
+    <row r="38" spans="2:8">
+      <c r="B38" s="11"/>
       <c r="C38" s="3" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="2:7">
-      <c r="B39" s="10"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+    <row r="39" spans="2:8">
+      <c r="B39" s="11"/>
+      <c r="C39" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="G39" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="11"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B35:B39"/>
+  <mergeCells count="7">
+    <mergeCell ref="F34:H35"/>
+    <mergeCell ref="B36:B40"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="B21:B25"/>
-    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="B28:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
updated lab addition to include ownersName
</commit_message>
<xml_diff>
--- a/updated_api_endpoints.xlsx
+++ b/updated_api_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\adv8\adv8_labOwners\labOwners3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F73B1F0-5BA6-4072-AD05-4F97F615E74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0E528A-8871-427F-882B-04EF636C6408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -339,12 +339,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -486,9 +493,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -499,10 +506,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -514,34 +521,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -819,7 +829,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:8" ht="90">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -837,7 +847,7 @@
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="12"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
@@ -851,7 +861,7 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="12"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
@@ -867,7 +877,7 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="12"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
@@ -883,7 +893,7 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="12"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
@@ -899,7 +909,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="90">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -919,7 +929,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="60">
-      <c r="B11" s="12"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
@@ -937,7 +947,7 @@
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="12"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
@@ -955,7 +965,7 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="12"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
@@ -971,7 +981,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="240">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="20" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -989,7 +999,7 @@
       </c>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="12"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
@@ -1003,7 +1013,7 @@
       </c>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="12"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1019,7 +1029,7 @@
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="12"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
@@ -1033,7 +1043,7 @@
       </c>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="12"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1047,7 +1057,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="300">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="20" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1068,7 +1078,7 @@
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="12"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="3" t="s">
         <v>11</v>
       </c>
@@ -1083,7 +1093,7 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="12"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1100,7 +1110,7 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="12"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="3" t="s">
         <v>35</v>
       </c>
@@ -1115,7 +1125,7 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="12"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="3" t="s">
         <v>36</v>
       </c>
@@ -1130,16 +1140,16 @@
       <c r="H25" s="3"/>
     </row>
     <row r="28" spans="2:8" ht="225">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="11" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="22" t="s">
         <v>47</v>
       </c>
       <c r="F28" s="2"/>
@@ -1151,8 +1161,8 @@
       </c>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="11"/>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="19"/>
+      <c r="C29" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -1165,8 +1175,8 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="11"/>
-      <c r="C30" s="13" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -1181,8 +1191,8 @@
       </c>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="11"/>
-      <c r="C31" s="13" t="s">
+      <c r="B31" s="19"/>
+      <c r="C31" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -1195,29 +1205,29 @@
       </c>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="11"/>
-      <c r="C32" s="14" t="s">
+      <c r="B32" s="19"/>
+      <c r="C32" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="15" t="s">
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="33" spans="2:8">
-      <c r="B33" s="11"/>
-      <c r="C33" s="21" t="s">
+      <c r="B33" s="19"/>
+      <c r="C33" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17" t="s">
+      <c r="E33" s="15"/>
+      <c r="F33" s="15" t="s">
         <v>53</v>
       </c>
       <c r="G33" s="10" t="s">
@@ -1236,11 +1246,11 @@
       <c r="E34" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F34" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
     </row>
     <row r="35" spans="2:8" ht="45">
       <c r="B35" s="3" t="s">
@@ -1251,9 +1261,9 @@
       <c r="E35" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
     </row>
     <row r="36" spans="2:8" ht="300">
       <c r="B36" s="18" t="s">
@@ -1270,7 +1280,7 @@
       </c>
     </row>
     <row r="37" spans="2:8">
-      <c r="B37" s="11"/>
+      <c r="B37" s="19"/>
       <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
@@ -1284,7 +1294,7 @@
       </c>
     </row>
     <row r="38" spans="2:8">
-      <c r="B38" s="11"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="3" t="s">
         <v>7</v>
       </c>
@@ -1300,7 +1310,7 @@
       </c>
     </row>
     <row r="39" spans="2:8">
-      <c r="B39" s="11"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="3" t="s">
         <v>35</v>
       </c>
@@ -1314,7 +1324,7 @@
       </c>
     </row>
     <row r="40" spans="2:8">
-      <c r="B40" s="11"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>

</xml_diff>

<commit_message>
updated labImageUrls in model
</commit_message>
<xml_diff>
--- a/updated_api_endpoints.xlsx
+++ b/updated_api_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\adv8\adv8_labOwners\labOwners3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0E528A-8871-427F-882B-04EF636C6408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BB7ACC-2B3A-4E64-9F85-51D363A28B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -783,7 +783,7 @@
   <dimension ref="B2:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
lab listing by ID is fixed
</commit_message>
<xml_diff>
--- a/updated_api_endpoints.xlsx
+++ b/updated_api_endpoints.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\adv8\adv8_labOwners\labOwners3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BB7ACC-2B3A-4E64-9F85-51D363A28B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912C7E25-71CA-4972-A642-892BF3FAA20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,25 +326,32 @@
     <t>updatedProduct JSON with ID</t>
   </si>
   <si>
-    <t>/getlab/owner</t>
-  </si>
-  <si>
     <t>Loggedin owners labs will be returned</t>
   </si>
   <si>
     <t>Will be implemented after lab onboarding and booking process starts</t>
+  </si>
+  <si>
+    <t>/lab/owner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -493,9 +500,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -506,10 +513,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -532,10 +539,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -547,12 +554,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,7 +791,7 @@
   <dimension ref="B2:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1149,7 +1157,7 @@
       <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="16" t="s">
         <v>47</v>
       </c>
       <c r="F28" s="2"/>
@@ -1220,15 +1228,15 @@
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="19"/>
-      <c r="C33" s="16" t="s">
-        <v>52</v>
+      <c r="C33" s="22" t="s">
+        <v>54</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E33" s="15"/>
-      <c r="F33" s="15" t="s">
-        <v>53</v>
+      <c r="F33" s="23" t="s">
+        <v>52</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>10</v>
@@ -1247,7 +1255,7 @@
         <v>41</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G34" s="17"/>
       <c r="H34" s="17"/>

</xml_diff>

<commit_message>
fixed add product issue
</commit_message>
<xml_diff>
--- a/updated_api_endpoints.xlsx
+++ b/updated_api_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\adv8\adv8_labOwners\labOwners3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912C7E25-71CA-4972-A642-892BF3FAA20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3580A92-B8CB-4136-AE8E-B06904927B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
   <si>
     <t>API Name</t>
   </si>
@@ -295,8 +295,26 @@
     </r>
   </si>
   <si>
+    <t>Yes, opened as of now</t>
+  </si>
+  <si>
+    <t>/api/product</t>
+  </si>
+  <si>
+    <t>updatedProduct JSON with ID</t>
+  </si>
+  <si>
+    <t>Loggedin owners labs will be returned</t>
+  </si>
+  <si>
+    <t>Will be implemented after lab onboarding and booking process starts</t>
+  </si>
+  <si>
+    <t>/lab/owner</t>
+  </si>
+  <si>
     <t>{
-  "labRef": "labID"
+  "labRef": "labID",
   "productList": [
     {
       "name": "Blood Test",
@@ -315,24 +333,6 @@
     }
   ]
 }</t>
-  </si>
-  <si>
-    <t>Yes, opened as of now</t>
-  </si>
-  <si>
-    <t>/api/product</t>
-  </si>
-  <si>
-    <t>updatedProduct JSON with ID</t>
-  </si>
-  <si>
-    <t>Loggedin owners labs will be returned</t>
-  </si>
-  <si>
-    <t>Will be implemented after lab onboarding and booking process starts</t>
-  </si>
-  <si>
-    <t>/lab/owner</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -522,9 +522,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -542,6 +539,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -557,10 +558,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -837,7 +840,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:8" ht="90">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -855,7 +858,7 @@
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="20"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
@@ -869,7 +872,7 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="20"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
@@ -885,7 +888,7 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="20"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
@@ -901,7 +904,7 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="20"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
@@ -917,7 +920,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="90">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -937,7 +940,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="60">
-      <c r="B11" s="20"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
@@ -955,7 +958,7 @@
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="20"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
@@ -973,7 +976,7 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="20"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
@@ -989,7 +992,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="240">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1007,7 +1010,7 @@
       </c>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="20"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
@@ -1021,7 +1024,7 @@
       </c>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="20"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1037,7 +1040,7 @@
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="20"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
@@ -1051,7 +1054,7 @@
       </c>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="20"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1065,7 +1068,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="300">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="21" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1086,7 +1089,7 @@
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="20"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="3" t="s">
         <v>11</v>
       </c>
@@ -1101,7 +1104,7 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="20"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1121,7 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="20"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="3" t="s">
         <v>35</v>
       </c>
@@ -1133,7 +1136,7 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="20"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="3" t="s">
         <v>36</v>
       </c>
@@ -1148,16 +1151,16 @@
       <c r="H25" s="3"/>
     </row>
     <row r="28" spans="2:8" ht="225">
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="15" t="s">
         <v>47</v>
       </c>
       <c r="F28" s="2"/>
@@ -1169,8 +1172,8 @@
       </c>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="19"/>
-      <c r="C29" s="11" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -1183,8 +1186,8 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="19"/>
-      <c r="C30" s="11" t="s">
+      <c r="B30" s="20"/>
+      <c r="C30" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -1199,8 +1202,8 @@
       </c>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="19"/>
-      <c r="C31" s="11" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -1213,35 +1216,35 @@
       </c>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="19"/>
-      <c r="C32" s="12" t="s">
+      <c r="B32" s="20"/>
+      <c r="C32" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="13" t="s">
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="33" spans="2:8">
-      <c r="B33" s="19"/>
-      <c r="C33" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="10" t="s">
+      <c r="B33" s="20"/>
+      <c r="C33" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="10" t="s">
+      <c r="E33" s="14"/>
+      <c r="F33" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1254,11 +1257,11 @@
       <c r="E34" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F34" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
+      <c r="F34" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
     </row>
     <row r="35" spans="2:8" ht="45">
       <c r="B35" s="3" t="s">
@@ -1269,26 +1272,29 @@
       <c r="E35" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
     </row>
     <row r="36" spans="2:8" ht="300">
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="G36" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="F36" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="37" spans="2:8">
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
@@ -1302,7 +1308,7 @@
       </c>
     </row>
     <row r="38" spans="2:8">
-      <c r="B38" s="19"/>
+      <c r="B38" s="20"/>
       <c r="C38" s="3" t="s">
         <v>7</v>
       </c>
@@ -1318,7 +1324,7 @@
       </c>
     </row>
     <row r="39" spans="2:8">
-      <c r="B39" s="19"/>
+      <c r="B39" s="20"/>
       <c r="C39" s="3" t="s">
         <v>35</v>
       </c>
@@ -1332,7 +1338,7 @@
       </c>
     </row>
     <row r="40" spans="2:8">
-      <c r="B40" s="19"/>
+      <c r="B40" s="20"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>

</xml_diff>

<commit_message>
OderAPI with Create, get, update and delete
</commit_message>
<xml_diff>
--- a/updated_api_endpoints.xlsx
+++ b/updated_api_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\adv8\adv8_labOwners\labOwners3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3580A92-B8CB-4136-AE8E-B06904927B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB575D9-62B1-4B55-8CF6-5D8A36E1E9B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="65">
   <si>
     <t>API Name</t>
   </si>
@@ -334,17 +334,96 @@
   ]
 }</t>
   </si>
+  <si>
+    <t>/api/order</t>
+  </si>
+  <si>
+    <t>/get/:orderId</t>
+  </si>
+  <si>
+    <t>/getUserOrders</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>/getLabOrders/:labID</t>
+  </si>
+  <si>
+    <t>/update/:orderId</t>
+  </si>
+  <si>
+    <t>/delete/:orderId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, </t>
+  </si>
+  <si>
+    <t>{ "userDetails": { "fullName": "Tuhin", "dateOfBirth": "2024-09-11", "gender": "male", "phoneNumber": "87968545543", "email": "tuhinmajumdar987@gmail.com", "address": "Kharagpur" }, "uploadedFiles": [ "https://firebasestorage.googleapis.com/v0/b/adva8-2023.appspot.com/o/medical_reports%2F46361.jpg?alt=media&amp;token=016f0051-44e6-428f-8b0b-cd90df5a3012" ], "selectedTests": [ { "id": 1, "name": "Blood Test", "description": "Complete blood count", "price": "$50" }, { "id": 3, "name": "X-Ray", "description": "Chest X-ray", "price": "$100" } ], "availability": { "day": "Wednesday", "timeSlot": "10AM - 11AM" }, "additionalFeatures": { "expressService": true, "onlineReports": false }, "totalTests": 2, "totalPrice": "150.00", "labRef": "66d06be03c5544e07b8b57eb" }</t>
+  </si>
+  <si>
+    <t>{
+    "userDetails": {
+        "fullName": "Tuhin",
+        "dateOfBirth": "2024-09-11",
+        "gender": "male",
+        "phoneNumber": "87968545543",
+        "email": "tuhinmajumdar987@gmail.com",
+        "address": "Kharagpur"
+    },
+    "uploadedFiles": [
+        "https://firebasestorage.googleapis.com/v0/b/adva8-2023.appspot.com/o/medical_reports%2F46361.jpg?alt=media&amp;token=016f0051-44e6-428f-8b0b-cd90df5a3012"
+    ],
+    "selectedTests": [
+        {
+            "id": 1,
+            "name": "Blood Test",
+            "description": "Complete blood count",
+            "price": "$50"
+        },
+        {
+            "id": 3,
+            "name": "X-Ray",
+            "description": "Chest X-ray",
+            "price": "$100"
+        }
+    ],
+    "availability": {
+        "day": "Wednesday",
+        "timeSlot": "10AM - 11AM"
+    },
+    "additionalFeatures": {
+        "expressService": true,
+        "onlineReports": false
+    },
+    "totalTests": 2,
+    "totalPrice": "150.00",
+    "labRef": "66d06be03c5544e07b8b57eb",
+    "userRef": "Dummy User",
+    "_id": "66fa68574f54396e02749557",
+    "createdAt": "2024-09-30T08:59:03.427Z",
+    "updatedAt": "2024-09-30T08:59:03.427Z",
+    "__v": 0
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -391,6 +470,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -412,7 +499,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -496,13 +583,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -513,10 +660,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -536,33 +683,72 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,19 +977,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H40"/>
+  <dimension ref="B2:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63.140625" customWidth="1"/>
-    <col min="6" max="6" width="44" customWidth="1"/>
+    <col min="6" max="6" width="67.7109375" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.140625" customWidth="1"/>
   </cols>
@@ -840,7 +1026,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:8" ht="90">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="23" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -858,7 +1044,7 @@
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="21"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
@@ -872,7 +1058,7 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="21"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
@@ -888,7 +1074,7 @@
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="21"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
@@ -904,7 +1090,7 @@
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="21"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
@@ -920,7 +1106,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="90">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="23" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -940,7 +1126,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="60">
-      <c r="B11" s="21"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
@@ -958,7 +1144,7 @@
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="21"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
@@ -976,7 +1162,7 @@
       </c>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="21"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
@@ -992,7 +1178,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="240">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="23" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1010,7 +1196,7 @@
       </c>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="21"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
@@ -1024,7 +1210,7 @@
       </c>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="21"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1040,7 +1226,7 @@
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="21"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
@@ -1054,7 +1240,7 @@
       </c>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="21"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1068,7 +1254,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" ht="300">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="23" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1089,7 +1275,7 @@
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="21"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="3" t="s">
         <v>11</v>
       </c>
@@ -1104,7 +1290,7 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="21"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1121,7 +1307,7 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="21"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="3" t="s">
         <v>35</v>
       </c>
@@ -1136,7 +1322,7 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="21"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="3" t="s">
         <v>36</v>
       </c>
@@ -1151,7 +1337,7 @@
       <c r="H25" s="3"/>
     </row>
     <row r="28" spans="2:8" ht="225">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="24" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -1172,7 +1358,7 @@
       </c>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="20"/>
+      <c r="B29" s="22"/>
       <c r="C29" s="10" t="s">
         <v>11</v>
       </c>
@@ -1186,7 +1372,7 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="20"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="10" t="s">
         <v>7</v>
       </c>
@@ -1202,7 +1388,7 @@
       </c>
     </row>
     <row r="31" spans="2:8">
-      <c r="B31" s="20"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="10" t="s">
         <v>35</v>
       </c>
@@ -1216,7 +1402,7 @@
       </c>
     </row>
     <row r="32" spans="2:8">
-      <c r="B32" s="20"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="11" t="s">
         <v>36</v>
       </c>
@@ -1230,7 +1416,7 @@
       </c>
     </row>
     <row r="33" spans="2:8">
-      <c r="B33" s="20"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="16" t="s">
         <v>53</v>
       </c>
@@ -1257,11 +1443,11 @@
       <c r="E34" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
     </row>
     <row r="35" spans="2:8" ht="45">
       <c r="B35" s="3" t="s">
@@ -1272,15 +1458,15 @@
       <c r="E35" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
     </row>
     <row r="36" spans="2:8" ht="300">
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="18" t="s">
         <v>32</v>
       </c>
       <c r="E36" s="5" t="s">
@@ -1289,12 +1475,12 @@
       <c r="F36" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G36" s="24" t="s">
+      <c r="G36" s="19" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="37" spans="2:8">
-      <c r="B37" s="20"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="3" t="s">
         <v>11</v>
       </c>
@@ -1308,7 +1494,7 @@
       </c>
     </row>
     <row r="38" spans="2:8">
-      <c r="B38" s="20"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="3" t="s">
         <v>7</v>
       </c>
@@ -1324,7 +1510,7 @@
       </c>
     </row>
     <row r="39" spans="2:8">
-      <c r="B39" s="20"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="3" t="s">
         <v>35</v>
       </c>
@@ -1338,15 +1524,100 @@
       </c>
     </row>
     <row r="40" spans="2:8">
-      <c r="B40" s="20"/>
+      <c r="B40" s="22"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
+    <row r="42" spans="2:8" ht="409.5">
+      <c r="B42" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="25"/>
+      <c r="C43" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="25"/>
+      <c r="C44" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="25"/>
+      <c r="C45" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="25"/>
+      <c r="C46" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="29"/>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="25"/>
+      <c r="C47" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="30"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="32"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="D46:G47"/>
     <mergeCell ref="F34:H35"/>
     <mergeCell ref="B36:B40"/>
     <mergeCell ref="B4:B8"/>

</xml_diff>